<commit_message>
dcp-624 - flatten spreadsheet with visium data
</commit_message>
<xml_diff>
--- a/scripts/metadata-spreadsheet-by-file/examples/RasaSpaceandTime250122_denormalised_Image-file_v0.3.xlsx
+++ b/scripts/metadata-spreadsheet-by-file/examples/RasaSpaceandTime250122_denormalised_Image-file_v0.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:JV4"/>
+  <dimension ref="A1:JH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>FILE NAME (Required)_Imaged specimen</t>
+          <t>FILE NAME (Required)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>FILE FORMAT (Required)_Imaged specimen</t>
+          <t>FILE FORMAT (Required)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CONTENT DESCRIPTION_Imaged specimen</t>
+          <t>CONTENT DESCRIPTION</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>CONTENT DESCRIPTION ONTOLOGY ID_Imaged specimen</t>
+          <t>CONTENT DESCRIPTION ONTOLOGY ID</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -461,12 +461,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>FILE SOURCE_Imaged specimen</t>
+          <t>FILE SOURCE</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>CHECKSUM_Imaged specimen</t>
+          <t>CHECKSUM</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -481,1362 +481,1292 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS ID (Required)_Image file</t>
+          <t>PROCESS ID (Required)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS NAME_Image file</t>
+          <t>PROCESS NAME</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS DESCRIPTION_Image file</t>
+          <t>PROCESS DESCRIPTION</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>LOCATION_Image file</t>
+          <t>LOCATION</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>OPERATOR(S)_Image file</t>
+          <t>OPERATOR(S)</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>START TIME (Required)_Image file</t>
+          <t>START TIME (Required)</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>END TIME_Image file</t>
+          <t>END TIME</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME_Image file</t>
+          <t>LENGTH OF TIME</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT_Image file</t>
+          <t>LENGTH OF TIME UNIT</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY ID_Image file</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Image file</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE (Required)_Image file</t>
+          <t>PROCESS TYPE (Required)</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE ONTOLOGY ID_Image file</t>
+          <t>PROCESS TYPE ONTOLOGY ID</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID_Image file</t>
+          <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>DEVIATION FROM PROTOCOL_Image file</t>
+          <t>DEVIATION FROM PROTOCOL</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>INSDC EXPERIMENT ACCESSION (Required)_Image file</t>
+          <t>INSDC EXPERIMENT ACCESSION (Required)</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
+          <t>ANALYSIS PROTOCOL ID (Required)</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
           <t>IMAGED SPECIMEN ID (Required)</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>IMAGED SPECIMEN NAME</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>IMAGED SPECIMEN DESCRIPTION</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>NCBI TAXON ID (Required)_Imaged Specimen</t>
-        </is>
-      </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>GENOTYPE_Imaged Specimen</t>
+          <t>NCBI TAXON ID (Required)</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>SUPPLEMENTARY FILES_Imaged Specimen</t>
+          <t>GENOTYPE</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>BIOSAMPLES ACCESSION_Imaged Specimen</t>
+          <t>SUPPLEMENTARY FILES</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>INSDC SAMPLE ACCESSION_Imaged Specimen</t>
+          <t>BIOSAMPLES ACCESSION</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>HDBR ACCESSION_Imaged Specimen</t>
+          <t>INSDC SAMPLE ACCESSION</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>GROSS IMAGE_Imaged Specimen</t>
+          <t>HDBR ACCESSION</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
+          <t>GROSS IMAGE</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
           <t>IMAGED SLICE THICKNESS (Required)</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>INTERNAL TISSUE STRUCTURES</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>INTERNAL TISSUE STRUCTURES ONTOLOGY ID</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>INTERNAL TISSUE STRUCTURES ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>INPUT SPECIMEN FROM ORGANISM ID (Required)</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>IMAGING PREPARATION PROTOCOL ID (Required)</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>PROCESS ID (Required)_Imaged specimen</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>PROCESS NAME_Imaged specimen</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>PROCESS DESCRIPTION_Imaged specimen</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>LOCATION_Imaged specimen</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>OPERATOR(S)_Imaged specimen</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>START TIME (Required)_Imaged specimen</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>END TIME_Imaged specimen</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>LENGTH OF TIME_Imaged specimen</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>LENGTH OF TIME UNIT_Imaged specimen</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>LENGTH OF TIME UNIT ONTOLOGY ID_Imaged specimen</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Imaged specimen</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>PROCESS TYPE (Required)_Imaged specimen</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>PROCESS TYPE ONTOLOGY ID_Imaged specimen</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID_Imaged specimen</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>DEVIATION FROM PROTOCOL_Imaged specimen</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>INSDC EXPERIMENT ACCESSION (Required)_Imaged specimen</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>IMAGING PROTOCOL NAME</t>
-        </is>
-      </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>IMAGING PROTOCOL DESCRIPTION</t>
+          <t>ANALYSIS PROTOCOL ID (Required)_Imaged specimen</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>PUBLICATION DOI_Imaged Specimen</t>
+          <t>SPECIMEN FROM ORGANISM ID (Required)</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>PROTOCOLS.IO DOI_Imaged Specimen</t>
+          <t>SPECIMEN FROM ORGANISM NAME</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>DOCUMENT FILENAME_Imaged Specimen</t>
+          <t>INPUT DONOR ORGANISM ID (Required)</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>MICROSCOPE SETUP DESCRIPTION</t>
+          <t>COLLECTION PROTOCOL ID (Required)</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>MICROSCOPY TECHNIQUE (Required)</t>
+          <t>SPECIMEN FROM ORGANISM DESCRIPTION</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>MICROSCOPY TECHNIQUE ONTOLOGY ID</t>
+          <t>NCBI TAXON ID (Required)_Specimen from organism</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>MICROSCOPY TECHNIQUE ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>GENOTYPE_Specimen from organism</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>MAGNIFICATION (Required)</t>
+          <t>SUPPLEMENTARY FILES_Specimen from organism</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL APERTURE (Required)</t>
+          <t>BIOSAMPLES ACCESSION_Specimen from organism</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>IMMERSION MEDIUM</t>
+          <t>INSDC SAMPLE ACCESSION_Specimen from organism</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>REFRACTIVE INDEX OF THE IMMERSION MEDIUM</t>
+          <t>HDBR ACCESSION_Specimen from organism</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>PIXEL SIZE (Required)</t>
+          <t>GENUS SPECIES (Required)</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>NUMBER OF TILES</t>
+          <t>GENUS SPECIES ONTOLOGY ID</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>TILE SIZE Y</t>
+          <t>GENUS SPECIES ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>TILE SIZE X</t>
+          <t>ORGAN (Required)</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>Z STACK STEP SIZE</t>
+          <t>ORGAN ONTOLOGY ID</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>NUMBER OF Z STEPS</t>
+          <t>ORGAN ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
-          <t>OVERLAPPING TILES (Required)</t>
+          <t>ORGAN PART</t>
         </is>
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>SPECIMEN FROM ORGANISM ID (Required)</t>
+          <t>ORGAN PART ONTOLOGY ID</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>SPECIMEN FROM ORGANISM NAME</t>
+          <t>ORGAN PART ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>INPUT DONOR ORGANISM ID (Required)</t>
+          <t>KNOWN DISEASE(S)</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>COLLECTION PROTOCOL ID (Required)</t>
+          <t>KNOWN DISEASE(S) ONTOLOGY ID</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>SPECIMEN FROM ORGANISM DESCRIPTION</t>
+          <t>KNOWN DISEASE(S) ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>NCBI TAXON ID (Required)_Specimen from organism</t>
+          <t>AUTOLYSIS SCORE</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>GENOTYPE_Specimen from organism</t>
+          <t>GROSS DESCRIPTION</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
         <is>
-          <t>SUPPLEMENTARY FILES_Specimen from organism</t>
+          <t>GROSS IMAGE_Specimen from organism</t>
         </is>
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>BIOSAMPLES ACCESSION_Specimen from organism</t>
+          <t>ISCHEMIC TEMPERATURE</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>INSDC SAMPLE ACCESSION_Specimen from organism</t>
+          <t>ISCHEMIC TIME</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>HDBR ACCESSION_Specimen from organism</t>
+          <t>MICROSCOPIC DESCRIPTION</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>GENUS SPECIES (Required)_Specimen from organism</t>
+          <t>MICROSCOPIC IMAGE</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>GENUS SPECIES ONTOLOGY ID_Specimen from organism</t>
+          <t>POST-MORTEM INTERVAL</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
         <is>
-          <t>GENUS SPECIES ONTOLOGY LABEL ONTOLOGY ID_Specimen from organism</t>
+          <t>STORAGE METHOD</t>
         </is>
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN (Required)</t>
+          <t>STORAGE TIME</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN ONTOLOGY ID</t>
+          <t>STORAGE TIME UNIT</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>STORAGE TIME UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN PART</t>
+          <t>STORAGE TIME UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN PART ONTOLOGY ID</t>
+          <t>PRESERVATION METHOD</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN PART ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>TIME OF COLLECTION</t>
         </is>
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>KNOWN DISEASE(S)_Specimen from organism</t>
+          <t>PURCHASED SPECIMEN - RETAIL NAME</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
         <is>
-          <t>KNOWN DISEASE(S) ONTOLOGY ID_Specimen from organism</t>
+          <t>PURCHASED SPECIMEN - CATALOG NUMBER</t>
         </is>
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>KNOWN DISEASE(S) ONTOLOGY LABEL ONTOLOGY ID_Specimen from organism</t>
+          <t>PURCHASED SPECIMEN - MANUFACTURER</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>AUTOLYSIS SCORE</t>
+          <t>PURCHASED SPECIMEN - BATCH/LOT NUMBER</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>GROSS DESCRIPTION</t>
+          <t>PURCHASED SPECIMEN - EXPIRY DATE</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>GROSS IMAGE_Specimen from organism</t>
+          <t>PURCHASED SPECIMEN - TITER</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>ISCHEMIC TEMPERATURE</t>
+          <t>PROCESS ID (Required)_Specimen from organism</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>ISCHEMIC TIME</t>
+          <t>PROCESS NAME_Specimen from organism</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>MICROSCOPIC DESCRIPTION</t>
+          <t>PROCESS DESCRIPTION_Specimen from organism</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>MICROSCOPIC IMAGE</t>
+          <t>LOCATION_Specimen from organism</t>
         </is>
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>POST-MORTEM INTERVAL</t>
+          <t>OPERATOR(S)_Specimen from organism</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE METHOD_Imaged Specimen</t>
+          <t>START TIME (Required)_Specimen from organism</t>
         </is>
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME_Imaged Specimen</t>
+          <t>END TIME_Specimen from organism</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME UNIT_Imaged Specimen</t>
+          <t>LENGTH OF TIME_Specimen from organism</t>
         </is>
       </c>
       <c r="DI1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME UNIT ONTOLOGY ID_Imaged Specimen</t>
+          <t>LENGTH OF TIME UNIT_Specimen from organism</t>
         </is>
       </c>
       <c r="DJ1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Imaged Specimen</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY ID_Specimen from organism</t>
         </is>
       </c>
       <c r="DK1" s="1" t="inlineStr">
         <is>
-          <t>PRESERVATION METHOD_Imaged Specimen</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Specimen from organism</t>
         </is>
       </c>
       <c r="DL1" s="1" t="inlineStr">
         <is>
-          <t>TIME OF COLLECTION</t>
+          <t>PROCESS TYPE (Required)_Specimen from organism</t>
         </is>
       </c>
       <c r="DM1" s="1" t="inlineStr">
         <is>
-          <t>PURCHASED SPECIMEN - RETAIL NAME</t>
+          <t>PROCESS TYPE ONTOLOGY ID_Specimen from organism</t>
         </is>
       </c>
       <c r="DN1" s="1" t="inlineStr">
         <is>
-          <t>PURCHASED SPECIMEN - CATALOG NUMBER</t>
+          <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID_Specimen from organism</t>
         </is>
       </c>
       <c r="DO1" s="1" t="inlineStr">
         <is>
-          <t>PURCHASED SPECIMEN - MANUFACTURER</t>
+          <t>DEVIATION FROM PROTOCOL_Specimen from organism</t>
         </is>
       </c>
       <c r="DP1" s="1" t="inlineStr">
         <is>
-          <t>PURCHASED SPECIMEN - BATCH/LOT NUMBER</t>
+          <t>INSDC EXPERIMENT ACCESSION (Required)_Specimen from organism</t>
         </is>
       </c>
       <c r="DQ1" s="1" t="inlineStr">
         <is>
-          <t>PURCHASED SPECIMEN - EXPIRY DATE</t>
+          <t>ANALYSIS PROTOCOL ID (Required)_Specimen from organism</t>
         </is>
       </c>
       <c r="DR1" s="1" t="inlineStr">
         <is>
-          <t>PURCHASED SPECIMEN - TITER</t>
+          <t>IMAGING PREPARATION PROTOCOL NAME</t>
         </is>
       </c>
       <c r="DS1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS ID (Required)_Specimen from organism</t>
+          <t>IMAGING PREPARATION PROTOCOL DESCRIPTION</t>
         </is>
       </c>
       <c r="DT1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS NAME_Specimen from organism</t>
+          <t>PUBLICATION DOI</t>
         </is>
       </c>
       <c r="DU1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS DESCRIPTION_Specimen from organism</t>
+          <t>PROTOCOLS.IO DOI</t>
         </is>
       </c>
       <c r="DV1" s="1" t="inlineStr">
         <is>
-          <t>LOCATION_Specimen from organism</t>
+          <t>DOCUMENT FILENAME</t>
         </is>
       </c>
       <c r="DW1" s="1" t="inlineStr">
         <is>
-          <t>OPERATOR(S)_Specimen from organism</t>
+          <t>FRESH SLICING METHOD</t>
         </is>
       </c>
       <c r="DX1" s="1" t="inlineStr">
         <is>
-          <t>START TIME (Required)_Specimen from organism</t>
+          <t>IMAGED SLICE THICKNESS</t>
         </is>
       </c>
       <c r="DY1" s="1" t="inlineStr">
         <is>
-          <t>END TIME_Specimen from organism</t>
+          <t>FINAL SLICING METHOD</t>
         </is>
       </c>
       <c r="DZ1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME_Specimen from organism</t>
+          <t>TIME BETWEEN RESECTION AND FRESH SLICING</t>
         </is>
       </c>
       <c r="EA1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT_Specimen from organism</t>
+          <t>POST RESECTION INTERVAL TIME UNIT</t>
         </is>
       </c>
       <c r="EB1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY ID_Specimen from organism</t>
+          <t>POST RESECTION INTERVAL TIME UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="EC1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Specimen from organism</t>
+          <t>POST RESECTION INTERVAL TIME UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="ED1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE (Required)_Specimen from organism</t>
+          <t>STORAGE METHOD_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EE1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE ONTOLOGY ID_Specimen from organism</t>
+          <t>STORAGE TIME_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EF1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID_Specimen from organism</t>
+          <t>STORAGE TIME UNIT_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EG1" s="1" t="inlineStr">
         <is>
-          <t>DEVIATION FROM PROTOCOL_Specimen from organism</t>
+          <t>STORAGE TIME UNIT ONTOLOGY ID_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EH1" s="1" t="inlineStr">
         <is>
-          <t>INSDC EXPERIMENT ACCESSION (Required)_Specimen from organism</t>
+          <t>STORAGE TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EI1" s="1" t="inlineStr">
         <is>
-          <t>IMAGING PREPARATION PROTOCOL NAME</t>
+          <t>PRESERVATION METHOD_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EJ1" s="1" t="inlineStr">
         <is>
-          <t>IMAGING PREPARATION PROTOCOL DESCRIPTION</t>
+          <t>POST FINAL SLICING INTERVAL</t>
         </is>
       </c>
       <c r="EK1" s="1" t="inlineStr">
         <is>
-          <t>PUBLICATION DOI_Imaging preparation protocol</t>
+          <t>POST FINAL SLICING INTERVAL TIME UNIT</t>
         </is>
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
-          <t>PROTOCOLS.IO DOI_Imaging preparation protocol</t>
+          <t>POST FINAL SLICING INTERVAL TIME UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="EM1" s="1" t="inlineStr">
         <is>
-          <t>DOCUMENT FILENAME_Imaging preparation protocol</t>
+          <t>POST FINAL SLICING INTERVAL TIME UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="EN1" s="1" t="inlineStr">
         <is>
-          <t>FRESH SLICING METHOD</t>
+          <t>FIDUCIAL MARKER</t>
         </is>
       </c>
       <c r="EO1" s="1" t="inlineStr">
         <is>
-          <t>IMAGED SLICE THICKNESS</t>
+          <t>EXPANSION FACTOR</t>
         </is>
       </c>
       <c r="EP1" s="1" t="inlineStr">
         <is>
-          <t>FINAL SLICING METHOD</t>
+          <t>ANALYSIS PROTOCOL ID (Required)_Imaging preparation protocol</t>
         </is>
       </c>
       <c r="EQ1" s="1" t="inlineStr">
         <is>
-          <t>TIME BETWEEN RESECTION AND FRESH SLICING</t>
+          <t>COLLECTION PROTOCOL NAME</t>
         </is>
       </c>
       <c r="ER1" s="1" t="inlineStr">
         <is>
-          <t>POST RESECTION INTERVAL TIME UNIT</t>
+          <t>COLLECTION PROTOCOL DESCRIPTION</t>
         </is>
       </c>
       <c r="ES1" s="1" t="inlineStr">
         <is>
-          <t>POST RESECTION INTERVAL TIME UNIT ONTOLOGY ID</t>
+          <t>PUBLICATION DOI_Collection protocol</t>
         </is>
       </c>
       <c r="ET1" s="1" t="inlineStr">
         <is>
-          <t>POST RESECTION INTERVAL TIME UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>PROTOCOLS.IO DOI_Collection protocol</t>
         </is>
       </c>
       <c r="EU1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE METHOD_Imaging preparation protocol</t>
+          <t>DOCUMENT FILENAME_Collection protocol</t>
         </is>
       </c>
       <c r="EV1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME_Imaging preparation protocol</t>
+          <t>COLLECTION METHOD (Required)</t>
         </is>
       </c>
       <c r="EW1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME UNIT_Imaging preparation protocol</t>
+          <t>COLLECTION METHOD ONTOLOGY ID</t>
         </is>
       </c>
       <c r="EX1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME UNIT ONTOLOGY ID_Imaging preparation protocol</t>
+          <t>COLLECTION METHOD ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="EY1" s="1" t="inlineStr">
         <is>
-          <t>STORAGE TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Imaging preparation protocol</t>
+          <t>RETAIL NAME</t>
         </is>
       </c>
       <c r="EZ1" s="1" t="inlineStr">
         <is>
-          <t>PRESERVATION METHOD_Imaging preparation protocol</t>
+          <t>CATALOG NUMBER</t>
         </is>
       </c>
       <c r="FA1" s="1" t="inlineStr">
         <is>
-          <t>POST FINAL SLICING INTERVAL</t>
+          <t>MANUFACTURER</t>
         </is>
       </c>
       <c r="FB1" s="1" t="inlineStr">
         <is>
-          <t>POST FINAL SLICING INTERVAL TIME UNIT</t>
+          <t>BATCH/LOT NUMBER</t>
         </is>
       </c>
       <c r="FC1" s="1" t="inlineStr">
         <is>
-          <t>POST FINAL SLICING INTERVAL TIME UNIT ONTOLOGY ID</t>
+          <t>EXPIRY DATE</t>
         </is>
       </c>
       <c r="FD1" s="1" t="inlineStr">
         <is>
-          <t>POST FINAL SLICING INTERVAL TIME UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>TITER</t>
         </is>
       </c>
       <c r="FE1" s="1" t="inlineStr">
         <is>
-          <t>FIDUCIAL MARKER</t>
+          <t>ANALYSIS PROTOCOL ID (Required)_Collection protocol</t>
         </is>
       </c>
       <c r="FF1" s="1" t="inlineStr">
         <is>
-          <t>EXPANSION FACTOR</t>
+          <t>DONOR ORGANISM ID (Required)</t>
         </is>
       </c>
       <c r="FG1" s="1" t="inlineStr">
         <is>
-          <t>COLLECTION PROTOCOL NAME</t>
+          <t>DONOR ORGANISM NAME</t>
         </is>
       </c>
       <c r="FH1" s="1" t="inlineStr">
         <is>
-          <t>COLLECTION PROTOCOL DESCRIPTION</t>
+          <t>DONOR ORGANISM DESCRIPTION</t>
         </is>
       </c>
       <c r="FI1" s="1" t="inlineStr">
         <is>
-          <t>PUBLICATION DOI</t>
+          <t>NCBI TAXON ID (Required)_Donor organism</t>
         </is>
       </c>
       <c r="FJ1" s="1" t="inlineStr">
         <is>
-          <t>PROTOCOLS.IO DOI</t>
+          <t>GENOTYPE_Donor organism</t>
         </is>
       </c>
       <c r="FK1" s="1" t="inlineStr">
         <is>
-          <t>DOCUMENT FILENAME</t>
+          <t>SUPPLEMENTARY FILES_Donor organism</t>
         </is>
       </c>
       <c r="FL1" s="1" t="inlineStr">
         <is>
-          <t>COLLECTION METHOD (Required)</t>
+          <t>BIOSAMPLES ACCESSION_Donor organism</t>
         </is>
       </c>
       <c r="FM1" s="1" t="inlineStr">
         <is>
-          <t>COLLECTION METHOD ONTOLOGY ID</t>
+          <t>INSDC SAMPLE ACCESSION_Donor organism</t>
         </is>
       </c>
       <c r="FN1" s="1" t="inlineStr">
         <is>
-          <t>COLLECTION METHOD ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>HDBR ACCESSION_Donor organism</t>
         </is>
       </c>
       <c r="FO1" s="1" t="inlineStr">
         <is>
-          <t>RETAIL NAME</t>
+          <t>BODY MASS INDEX</t>
         </is>
       </c>
       <c r="FP1" s="1" t="inlineStr">
         <is>
-          <t>CATALOG NUMBER</t>
+          <t>ETHNICITY</t>
         </is>
       </c>
       <c r="FQ1" s="1" t="inlineStr">
         <is>
-          <t>MANUFACTURER</t>
+          <t>ETHNICITY ONTOLOGY ID</t>
         </is>
       </c>
       <c r="FR1" s="1" t="inlineStr">
         <is>
-          <t>BATCH/LOT NUMBER</t>
+          <t>ETHNICITY ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="FS1" s="1" t="inlineStr">
         <is>
-          <t>EXPIRY DATE</t>
+          <t>MOUSE STRAIN</t>
         </is>
       </c>
       <c r="FT1" s="1" t="inlineStr">
         <is>
-          <t>TITER</t>
+          <t>MOUSE STRAIN ONTOLOGY ID</t>
         </is>
       </c>
       <c r="FU1" s="1" t="inlineStr">
         <is>
-          <t>DONOR ORGANISM ID (Required)</t>
+          <t>MOUSE STRAIN ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="FV1" s="1" t="inlineStr">
         <is>
-          <t>DONOR ORGANISM NAME</t>
+          <t>GENUS SPECIES (Required)_Donor organism</t>
         </is>
       </c>
       <c r="FW1" s="1" t="inlineStr">
         <is>
-          <t>DONOR ORGANISM DESCRIPTION</t>
+          <t>GENUS SPECIES ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="FX1" s="1" t="inlineStr">
         <is>
-          <t>NCBI TAXON ID (Required)</t>
+          <t>GENUS SPECIES ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="FY1" s="1" t="inlineStr">
         <is>
-          <t>GENOTYPE</t>
+          <t>BIOLOGICAL SEX (Required)</t>
         </is>
       </c>
       <c r="FZ1" s="1" t="inlineStr">
         <is>
-          <t>SUPPLEMENTARY FILES</t>
+          <t>ALIVE AT COLLECTION (Required)</t>
         </is>
       </c>
       <c r="GA1" s="1" t="inlineStr">
         <is>
-          <t>BIOSAMPLES ACCESSION</t>
+          <t>AGE</t>
         </is>
       </c>
       <c r="GB1" s="1" t="inlineStr">
         <is>
-          <t>INSDC SAMPLE ACCESSION</t>
+          <t>AGE UNIT</t>
         </is>
       </c>
       <c r="GC1" s="1" t="inlineStr">
         <is>
-          <t>HDBR ACCESSION</t>
+          <t>AGE UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="GD1" s="1" t="inlineStr">
         <is>
-          <t>BODY MASS INDEX</t>
+          <t>AGE UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="GE1" s="1" t="inlineStr">
         <is>
-          <t>ETHNICITY</t>
+          <t>DEVELOPMENT STAGE (Required)</t>
         </is>
       </c>
       <c r="GF1" s="1" t="inlineStr">
         <is>
-          <t>ETHNICITY ONTOLOGY ID</t>
+          <t>DEVELOPMENT STAGE ONTOLOGY ID</t>
         </is>
       </c>
       <c r="GG1" s="1" t="inlineStr">
         <is>
-          <t>ETHNICITY ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>DEVELOPMENT STAGE ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="GH1" s="1" t="inlineStr">
         <is>
-          <t>MOUSE STRAIN</t>
+          <t>KNOWN DISEASE(S)_Donor organism</t>
         </is>
       </c>
       <c r="GI1" s="1" t="inlineStr">
         <is>
-          <t>MOUSE STRAIN ONTOLOGY ID</t>
+          <t>KNOWN DISEASE(S) ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="GJ1" s="1" t="inlineStr">
         <is>
-          <t>MOUSE STRAIN ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>KNOWN DISEASE(S) ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="GK1" s="1" t="inlineStr">
         <is>
-          <t>GENUS SPECIES (Required)_Donor organism</t>
+          <t>CAUSE OF DEATH (Required)</t>
         </is>
       </c>
       <c r="GL1" s="1" t="inlineStr">
         <is>
-          <t>GENUS SPECIES ONTOLOGY ID_Donor organism</t>
+          <t>COLD PERFUSED</t>
         </is>
       </c>
       <c r="GM1" s="1" t="inlineStr">
         <is>
-          <t>GENUS SPECIES ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
+          <t>NUMBER OF DAYS ON VENTILATOR</t>
         </is>
       </c>
       <c r="GN1" s="1" t="inlineStr">
         <is>
-          <t>BIOLOGICAL SEX (Required)</t>
+          <t>VALUE ON HARDY SCALE</t>
         </is>
       </c>
       <c r="GO1" s="1" t="inlineStr">
         <is>
-          <t>ALIVE AT COLLECTION (Required)</t>
+          <t>TIME OF DEATH</t>
         </is>
       </c>
       <c r="GP1" s="1" t="inlineStr">
         <is>
-          <t>AGE</t>
+          <t>ORGAN DONATION DEATH TYPE</t>
         </is>
       </c>
       <c r="GQ1" s="1" t="inlineStr">
         <is>
-          <t>AGE UNIT</t>
+          <t>NORMOTHERMIC REGIONAL PERFUSION</t>
         </is>
       </c>
       <c r="GR1" s="1" t="inlineStr">
         <is>
-          <t>AGE UNIT ONTOLOGY ID</t>
+          <t>ALCOHOL HISTORY</t>
         </is>
       </c>
       <c r="GS1" s="1" t="inlineStr">
         <is>
-          <t>AGE UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>MEDICATIONS</t>
         </is>
       </c>
       <c r="GT1" s="1" t="inlineStr">
         <is>
-          <t>DEVELOPMENT STAGE (Required)</t>
+          <t>SMOKING HISTORY</t>
         </is>
       </c>
       <c r="GU1" s="1" t="inlineStr">
         <is>
-          <t>DEVELOPMENT STAGE ONTOLOGY ID</t>
+          <t>NUTRITIONAL STATE</t>
         </is>
       </c>
       <c r="GV1" s="1" t="inlineStr">
         <is>
-          <t>DEVELOPMENT STAGE ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>TEST RESULTS</t>
         </is>
       </c>
       <c r="GW1" s="1" t="inlineStr">
         <is>
-          <t>KNOWN DISEASE(S)_Donor organism</t>
+          <t>TREATMENTS</t>
         </is>
       </c>
       <c r="GX1" s="1" t="inlineStr">
         <is>
-          <t>KNOWN DISEASE(S) ONTOLOGY ID_Donor organism</t>
+          <t>GESTATIONAL AGE</t>
         </is>
       </c>
       <c r="GY1" s="1" t="inlineStr">
         <is>
-          <t>KNOWN DISEASE(S) ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
+          <t>GESTATIONAL AGE UNIT</t>
         </is>
       </c>
       <c r="GZ1" s="1" t="inlineStr">
         <is>
-          <t>CAUSE OF DEATH (Required)</t>
+          <t>GESTATIONAL AGE UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HA1" s="1" t="inlineStr">
         <is>
-          <t>COLD PERFUSED</t>
+          <t>GESTATIONAL AGE UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HB1" s="1" t="inlineStr">
         <is>
-          <t>NUMBER OF DAYS ON VENTILATOR</t>
+          <t>HEIGHT</t>
         </is>
       </c>
       <c r="HC1" s="1" t="inlineStr">
         <is>
-          <t>VALUE ON HARDY SCALE</t>
+          <t>HEIGHT UNIT</t>
         </is>
       </c>
       <c r="HD1" s="1" t="inlineStr">
         <is>
-          <t>TIME OF DEATH</t>
+          <t>HEIGHT UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HE1" s="1" t="inlineStr">
         <is>
-          <t>ORGAN DONATION DEATH TYPE</t>
+          <t>HEIGHT UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HF1" s="1" t="inlineStr">
         <is>
-          <t>NORMOTHERMIC REGIONAL PERFUSION</t>
+          <t>WEIGHT</t>
         </is>
       </c>
       <c r="HG1" s="1" t="inlineStr">
         <is>
-          <t>ALCOHOL HISTORY</t>
+          <t>WEIGHT UNIT</t>
         </is>
       </c>
       <c r="HH1" s="1" t="inlineStr">
         <is>
-          <t>MEDICATIONS</t>
+          <t>WEIGHT UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HI1" s="1" t="inlineStr">
         <is>
-          <t>SMOKING HISTORY</t>
+          <t>WEIGHT UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HJ1" s="1" t="inlineStr">
         <is>
-          <t>NUTRITIONAL STATE</t>
+          <t>TIMECOURSE VALUE (Required)</t>
         </is>
       </c>
       <c r="HK1" s="1" t="inlineStr">
         <is>
-          <t>TEST RESULTS</t>
+          <t>TIMECOURSE UNIT (Required)</t>
         </is>
       </c>
       <c r="HL1" s="1" t="inlineStr">
         <is>
-          <t>TREATMENTS</t>
+          <t>TIMECOURSE UNIT ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HM1" s="1" t="inlineStr">
         <is>
-          <t>GESTATIONAL AGE</t>
+          <t>TIMECOURSE UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
         </is>
       </c>
       <c r="HN1" s="1" t="inlineStr">
         <is>
-          <t>GESTATIONAL AGE UNIT</t>
+          <t>TIMECOURSE RELEVANCE</t>
         </is>
       </c>
       <c r="HO1" s="1" t="inlineStr">
         <is>
-          <t>GESTATIONAL AGE UNIT ONTOLOGY ID</t>
+          <t>PROCESS ID (Required)_Donor organism</t>
         </is>
       </c>
       <c r="HP1" s="1" t="inlineStr">
         <is>
-          <t>GESTATIONAL AGE UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>PROCESS NAME_Donor organism</t>
         </is>
       </c>
       <c r="HQ1" s="1" t="inlineStr">
         <is>
-          <t>HEIGHT</t>
+          <t>PROCESS DESCRIPTION_Donor organism</t>
         </is>
       </c>
       <c r="HR1" s="1" t="inlineStr">
         <is>
-          <t>HEIGHT UNIT</t>
+          <t>LOCATION_Donor organism</t>
         </is>
       </c>
       <c r="HS1" s="1" t="inlineStr">
         <is>
-          <t>HEIGHT UNIT ONTOLOGY ID</t>
+          <t>OPERATOR(S)_Donor organism</t>
         </is>
       </c>
       <c r="HT1" s="1" t="inlineStr">
         <is>
-          <t>HEIGHT UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>START TIME (Required)_Donor organism</t>
         </is>
       </c>
       <c r="HU1" s="1" t="inlineStr">
         <is>
-          <t>WEIGHT</t>
+          <t>END TIME_Donor organism</t>
         </is>
       </c>
       <c r="HV1" s="1" t="inlineStr">
         <is>
-          <t>WEIGHT UNIT</t>
+          <t>LENGTH OF TIME_Donor organism</t>
         </is>
       </c>
       <c r="HW1" s="1" t="inlineStr">
         <is>
-          <t>WEIGHT UNIT ONTOLOGY ID</t>
+          <t>LENGTH OF TIME UNIT_Donor organism</t>
         </is>
       </c>
       <c r="HX1" s="1" t="inlineStr">
         <is>
-          <t>WEIGHT UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="HY1" s="1" t="inlineStr">
         <is>
-          <t>TIMECOURSE VALUE (Required)</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="HZ1" s="1" t="inlineStr">
         <is>
-          <t>TIMECOURSE UNIT (Required)</t>
+          <t>PROCESS TYPE (Required)_Donor organism</t>
         </is>
       </c>
       <c r="IA1" s="1" t="inlineStr">
         <is>
-          <t>TIMECOURSE UNIT ONTOLOGY ID</t>
+          <t>PROCESS TYPE ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="IB1" s="1" t="inlineStr">
         <is>
-          <t>TIMECOURSE UNIT ONTOLOGY LABEL ONTOLOGY ID</t>
+          <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
         </is>
       </c>
       <c r="IC1" s="1" t="inlineStr">
         <is>
-          <t>TIMECOURSE RELEVANCE</t>
+          <t>DEVIATION FROM PROTOCOL_Donor organism</t>
         </is>
       </c>
       <c r="ID1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS ID (Required)_Donor organism</t>
+          <t>INSDC EXPERIMENT ACCESSION (Required)_Donor organism</t>
         </is>
       </c>
       <c r="IE1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS NAME_Donor organism</t>
+          <t>ANALYSIS PROTOCOL ID (Required)_Donor organism</t>
         </is>
       </c>
       <c r="IF1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS DESCRIPTION_Donor organism</t>
+          <t>FILE NAME (Required)_Analysis file</t>
         </is>
       </c>
       <c r="IG1" s="1" t="inlineStr">
         <is>
-          <t>LOCATION_Donor organism</t>
+          <t>FILE FORMAT (Required)_Analysis file</t>
         </is>
       </c>
       <c r="IH1" s="1" t="inlineStr">
         <is>
-          <t>OPERATOR(S)_Donor organism</t>
+          <t>CONTENT DESCRIPTION_Analysis file</t>
         </is>
       </c>
       <c r="II1" s="1" t="inlineStr">
         <is>
-          <t>START TIME (Required)_Donor organism</t>
+          <t>CONTENT DESCRIPTION ONTOLOGY ID_Analysis file</t>
         </is>
       </c>
       <c r="IJ1" s="1" t="inlineStr">
         <is>
-          <t>END TIME_Donor organism</t>
+          <t>CONTENT DESCRIPTION ONTOLOGY LABEL</t>
         </is>
       </c>
       <c r="IK1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME_Donor organism</t>
+          <t>CHECKSUM_Analysis file</t>
         </is>
       </c>
       <c r="IL1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT_Donor organism</t>
+          <t>FILE SOURCE_Analysis file</t>
         </is>
       </c>
       <c r="IM1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY ID_Donor organism</t>
+          <t>MATRIX CELL COUNT</t>
         </is>
       </c>
       <c r="IN1" s="1" t="inlineStr">
         <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
+          <t>ANALYSIS PROTOCOL ID (Required)_Analysis file</t>
         </is>
       </c>
       <c r="IO1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE (Required)_Donor organism</t>
+          <t>CELL SUSPENSION ID (Required)</t>
         </is>
       </c>
       <c r="IP1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE ONTOLOGY ID_Donor organism</t>
+          <t>LIBRARY PREPARATION PROTOCOL ID (Required)</t>
         </is>
       </c>
       <c r="IQ1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS TYPE ONTOLOGY LABEL ONTOLOGY ID_Donor organism</t>
+          <t>SEQUENCING PROTOCOL ID (Required)</t>
         </is>
       </c>
       <c r="IR1" s="1" t="inlineStr">
         <is>
-          <t>DEVIATION FROM PROTOCOL_Donor organism</t>
+          <t>IMAGING PROTOCOL (Required)</t>
         </is>
       </c>
       <c r="IS1" s="1" t="inlineStr">
         <is>
-          <t>INSDC EXPERIMENT ACCESSION (Required)_Donor organism</t>
+          <t>PROCESS ID (Required)_Analysis file</t>
         </is>
       </c>
       <c r="IT1" s="1" t="inlineStr">
         <is>
-          <t>FILE NAME (Required)_Analysis file</t>
+          <t>PROCESS NAME_Analysis file</t>
         </is>
       </c>
       <c r="IU1" s="1" t="inlineStr">
         <is>
-          <t>FILE FORMAT (Required)_Analysis file</t>
+          <t>PROCESS DESCRIPTION_Analysis file</t>
         </is>
       </c>
       <c r="IV1" s="1" t="inlineStr">
         <is>
-          <t>CONTENT DESCRIPTION_Analysis file</t>
+          <t>LOCATION_Analysis file</t>
         </is>
       </c>
       <c r="IW1" s="1" t="inlineStr">
         <is>
-          <t>CONTENT DESCRIPTION ONTOLOGY ID_Analysis file</t>
+          <t>OPERATOR(S)_Analysis file</t>
         </is>
       </c>
       <c r="IX1" s="1" t="inlineStr">
         <is>
-          <t>CONTENT DESCRIPTION ONTOLOGY LABEL</t>
+          <t>START TIME</t>
         </is>
       </c>
       <c r="IY1" s="1" t="inlineStr">
         <is>
-          <t>CHECKSUM_Analysis file</t>
+          <t>END TIME_Analysis file</t>
         </is>
       </c>
       <c r="IZ1" s="1" t="inlineStr">
         <is>
-          <t>FILE SOURCE_Analysis file</t>
+          <t>LENGTH OF TIME_Analysis file</t>
         </is>
       </c>
       <c r="JA1" s="1" t="inlineStr">
         <is>
-          <t>MATRIX CELL COUNT</t>
+          <t>LENGTH OF TIME UNIT_Analysis file</t>
         </is>
       </c>
       <c r="JB1" s="1" t="inlineStr">
         <is>
-          <t>ANALYSIS PROTOCOL ID (Required)</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY ID_Analysis file</t>
         </is>
       </c>
       <c r="JC1" s="1" t="inlineStr">
         <is>
-          <t>CELL SUSPENSION ID (Required)</t>
+          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL</t>
         </is>
       </c>
       <c r="JD1" s="1" t="inlineStr">
         <is>
-          <t>LIBRARY PREPARATION PROTOCOL ID (Required)</t>
+          <t>PROCESS TYPE</t>
         </is>
       </c>
       <c r="JE1" s="1" t="inlineStr">
         <is>
-          <t>SEQUENCING PROTOCOL ID (Required)</t>
+          <t>PROCESS TYPE ONTOLOGY ID_Analysis file</t>
         </is>
       </c>
       <c r="JF1" s="1" t="inlineStr">
         <is>
-          <t>IMAGING PROTOCOL (Required)</t>
+          <t>PROCESS TYPE ONTOLOGY LABEL</t>
         </is>
       </c>
       <c r="JG1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS ID (Required)</t>
+          <t>DEVIATION FROM PROTOCOL_Analysis file</t>
         </is>
       </c>
       <c r="JH1" s="1" t="inlineStr">
         <is>
-          <t>PROCESS NAME</t>
-        </is>
-      </c>
-      <c r="JI1" s="1" t="inlineStr">
-        <is>
-          <t>PROCESS DESCRIPTION</t>
-        </is>
-      </c>
-      <c r="JJ1" s="1" t="inlineStr">
-        <is>
-          <t>LOCATION</t>
-        </is>
-      </c>
-      <c r="JK1" s="1" t="inlineStr">
-        <is>
-          <t>OPERATOR(S)</t>
-        </is>
-      </c>
-      <c r="JL1" s="1" t="inlineStr">
-        <is>
-          <t>START TIME</t>
-        </is>
-      </c>
-      <c r="JM1" s="1" t="inlineStr">
-        <is>
-          <t>END TIME</t>
-        </is>
-      </c>
-      <c r="JN1" s="1" t="inlineStr">
-        <is>
-          <t>LENGTH OF TIME</t>
-        </is>
-      </c>
-      <c r="JO1" s="1" t="inlineStr">
-        <is>
-          <t>LENGTH OF TIME UNIT</t>
-        </is>
-      </c>
-      <c r="JP1" s="1" t="inlineStr">
-        <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY ID</t>
-        </is>
-      </c>
-      <c r="JQ1" s="1" t="inlineStr">
-        <is>
-          <t>LENGTH OF TIME UNIT ONTOLOGY LABEL</t>
-        </is>
-      </c>
-      <c r="JR1" s="1" t="inlineStr">
-        <is>
-          <t>PROCESS TYPE</t>
-        </is>
-      </c>
-      <c r="JS1" s="1" t="inlineStr">
-        <is>
-          <t>PROCESS TYPE ONTOLOGY ID</t>
-        </is>
-      </c>
-      <c r="JT1" s="1" t="inlineStr">
-        <is>
-          <t>PROCESS TYPE ONTOLOGY LABEL</t>
-        </is>
-      </c>
-      <c r="JU1" s="1" t="inlineStr">
-        <is>
-          <t>DEVIATION FROM PROTOCOL</t>
-        </is>
-      </c>
-      <c r="JV1" s="1" t="inlineStr">
-        <is>
-          <t>INSDC EXPERIMENT ACCESSION (Required)</t>
+          <t>INSDC EXPERIMENT ACCESSION (Required)_Analysis file</t>
         </is>
       </c>
     </row>
@@ -1886,301 +1816,245 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
+          <t>['6330STDY9479159imagespecimen']</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
           <t>6330STDY9479159imagespecimen</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>6330STDY9479159imagespecimen</t>
         </is>
       </c>
-      <c r="AD2" t="n">
+      <c r="AE2" t="n">
         <v>9606</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AL2" t="n">
         <v>10</v>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>6330STDY9479159specimen</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>HumanVisiumSpatialLibraryPrep</t>
         </is>
       </c>
-      <c r="BG2" t="inlineStr">
-        <is>
-          <t>VisiumImagingProtocol</t>
-        </is>
-      </c>
       <c r="BH2" t="inlineStr">
         <is>
-          <t>All images for this process were scanned x40 on Hamamatsu NanoZoomer S60.</t>
+          <t>['6330STDY9479159imagespecimen']</t>
+        </is>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>6330STDY9479159specimen</t>
+        </is>
+      </c>
+      <c r="BJ2" t="inlineStr">
+        <is>
+          <t>HumanFetalVisium</t>
+        </is>
+      </c>
+      <c r="BK2" t="inlineStr">
+        <is>
+          <t>F78-14789</t>
+        </is>
+      </c>
+      <c r="BL2" t="inlineStr">
+        <is>
+          <t>HumanVisiumCollection</t>
         </is>
       </c>
       <c r="BM2" t="inlineStr">
         <is>
-          <t>fluorescence microscopy</t>
-        </is>
-      </c>
-      <c r="BN2" t="inlineStr">
-        <is>
-          <t>FBbi:00000246</t>
-        </is>
-      </c>
-      <c r="BO2" t="inlineStr">
-        <is>
-          <t>fluorescence microscopy</t>
-        </is>
-      </c>
-      <c r="BP2" t="inlineStr">
-        <is>
-          <t>40x</t>
-        </is>
-      </c>
-      <c r="BQ2" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="BT2" t="n">
-        <v>230</v>
+          <t>F78-FTIL-0-FO-4-S4</t>
+        </is>
+      </c>
+      <c r="BN2" t="n">
+        <v>9606</v>
+      </c>
+      <c r="BT2" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>NCBITaxon:9606</t>
+        </is>
+      </c>
+      <c r="BV2" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>small intestine</t>
+        </is>
+      </c>
+      <c r="BX2" t="inlineStr">
+        <is>
+          <t>UBERON:0002108</t>
+        </is>
+      </c>
+      <c r="BY2" t="inlineStr">
+        <is>
+          <t>small intestine</t>
+        </is>
       </c>
       <c r="BZ2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>terminal ileum</t>
         </is>
       </c>
       <c r="CA2" t="inlineStr">
         <is>
-          <t>6330STDY9479159specimen</t>
+          <t>FMA:14966</t>
         </is>
       </c>
       <c r="CB2" t="inlineStr">
         <is>
-          <t>HumanFetalVisium</t>
-        </is>
-      </c>
-      <c r="CC2" t="inlineStr">
+          <t>Distal part of ileum</t>
+        </is>
+      </c>
+      <c r="DQ2" t="inlineStr">
+        <is>
+          <t>['6330STDY9479159specimen']</t>
+        </is>
+      </c>
+      <c r="DS2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> All tissues were sectioned using the Leica CX3050S cryostat and were cut at 10um. Tissue optimization was performed to obtain permeabilization time for fetal tissue (12 min).</t>
+        </is>
+      </c>
+      <c r="EP2" t="inlineStr">
+        <is>
+          <t>['HumanVisiumSpatialLibraryPrep']</t>
+        </is>
+      </c>
+      <c r="ER2" t="inlineStr">
+        <is>
+          <t>Human fetal tissues were obtained from the MRC/Wellcome Trust-funded Human Developmental Biology Resource(HDBR, http://www.hdbr.org) with appropriate maternal written consent and approval from the Newcastle and North Tyneside NHS Health Authority Joint Ethics Committee (08/H0906/21+5). All tissues were processed immediately after isolation using consistent protocols with variation in enzymatic digestion strength. Samples were embedded in OCT, either in a mould or on a piece of cork, either over dry ice or in a liquid nitrogen bath.</t>
+        </is>
+      </c>
+      <c r="EV2" t="inlineStr">
+        <is>
+          <t>collecting specimen from organ postmortem</t>
+        </is>
+      </c>
+      <c r="EW2" t="inlineStr">
+        <is>
+          <t>EFO:0009627</t>
+        </is>
+      </c>
+      <c r="EX2" t="inlineStr">
+        <is>
+          <t>collecting specimen from organ postmortem</t>
+        </is>
+      </c>
+      <c r="FE2" t="inlineStr">
+        <is>
+          <t>['HumanVisiumCollection']</t>
+        </is>
+      </c>
+      <c r="FF2" t="inlineStr">
         <is>
           <t>F78-14789</t>
         </is>
       </c>
-      <c r="CD2" t="inlineStr">
-        <is>
-          <t>HumanVisiumCollection</t>
-        </is>
-      </c>
-      <c r="CE2" t="inlineStr">
-        <is>
-          <t>F78-FTIL-0-FO-4-S4</t>
-        </is>
-      </c>
-      <c r="CF2" t="n">
+      <c r="FG2" t="inlineStr">
+        <is>
+          <t>HumanFetal</t>
+        </is>
+      </c>
+      <c r="FI2" t="n">
         <v>9606</v>
       </c>
-      <c r="CL2" t="inlineStr">
+      <c r="FN2" t="n">
+        <v>14789</v>
+      </c>
+      <c r="FV2" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="CM2" t="inlineStr">
+      <c r="FW2" t="inlineStr">
         <is>
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="CN2" t="inlineStr">
+      <c r="FX2" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="CO2" t="inlineStr">
-        <is>
-          <t>small intestine</t>
-        </is>
-      </c>
-      <c r="CP2" t="inlineStr">
-        <is>
-          <t>UBERON:0002108</t>
-        </is>
-      </c>
-      <c r="CQ2" t="inlineStr">
-        <is>
-          <t>small intestine</t>
-        </is>
-      </c>
-      <c r="CR2" t="inlineStr">
-        <is>
-          <t>terminal ileum</t>
-        </is>
-      </c>
-      <c r="CS2" t="inlineStr">
-        <is>
-          <t>FMA:14966</t>
-        </is>
-      </c>
-      <c r="CT2" t="inlineStr">
-        <is>
-          <t>Distal part of ileum</t>
-        </is>
-      </c>
-      <c r="EJ2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> All tissues were sectioned using the Leica CX3050S cryostat and were cut at 10um. Tissue optimization was performed to obtain permeabilization time for fetal tissue (12 min).</t>
-        </is>
-      </c>
-      <c r="FH2" t="inlineStr">
-        <is>
-          <t>Human fetal tissues were obtained from the MRC/Wellcome Trust-funded Human Developmental Biology Resource(HDBR, http://www.hdbr.org) with appropriate maternal written consent and approval from the Newcastle and North Tyneside NHS Health Authority Joint Ethics Committee (08/H0906/21+5). All tissues were processed immediately after isolation using consistent protocols with variation in enzymatic digestion strength. Samples were embedded in OCT, either in a mould or on a piece of cork, either over dry ice or in a liquid nitrogen bath.</t>
-        </is>
-      </c>
-      <c r="FL2" t="inlineStr">
-        <is>
-          <t>collecting specimen from organ postmortem</t>
-        </is>
-      </c>
-      <c r="FM2" t="inlineStr">
-        <is>
-          <t>EFO:0009627</t>
-        </is>
-      </c>
-      <c r="FN2" t="inlineStr">
-        <is>
-          <t>collecting specimen from organ postmortem</t>
-        </is>
-      </c>
-      <c r="FU2" t="inlineStr">
-        <is>
-          <t>F78-14789</t>
-        </is>
-      </c>
-      <c r="FV2" t="inlineStr">
-        <is>
-          <t>HumanFetal</t>
-        </is>
-      </c>
-      <c r="FX2" t="n">
-        <v>9606</v>
-      </c>
-      <c r="GC2" t="n">
-        <v>14789</v>
-      </c>
-      <c r="GK2" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="GL2" t="inlineStr">
-        <is>
-          <t>NCBITaxon:9606</t>
-        </is>
-      </c>
-      <c r="GM2" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="GN2" t="inlineStr">
+      <c r="FY2" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="GO2" t="inlineStr">
+      <c r="FZ2" t="inlineStr">
         <is>
           <t>not applicable</t>
         </is>
       </c>
-      <c r="GT2" t="inlineStr">
+      <c r="GE2" t="inlineStr">
         <is>
           <t>embryo</t>
         </is>
       </c>
-      <c r="GU2" t="inlineStr">
+      <c r="GF2" t="inlineStr">
         <is>
           <t>UBERON:0000068</t>
         </is>
       </c>
-      <c r="GV2" t="inlineStr">
+      <c r="GG2" t="inlineStr">
         <is>
           <t>embryo stage</t>
         </is>
       </c>
-      <c r="GW2" t="inlineStr">
+      <c r="GH2" t="inlineStr">
         <is>
           <t>normal</t>
         </is>
       </c>
-      <c r="GX2" t="inlineStr">
+      <c r="GI2" t="inlineStr">
         <is>
           <t>PATO:0000461</t>
         </is>
       </c>
+      <c r="GJ2" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="GX2" t="n">
+        <v>17</v>
+      </c>
       <c r="GY2" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="HM2" t="n">
-        <v>17</v>
-      </c>
-      <c r="HN2" t="inlineStr">
-        <is>
           <t>week</t>
         </is>
       </c>
-      <c r="HO2" t="inlineStr">
+      <c r="GZ2" t="inlineStr">
         <is>
           <t>UO:0000034</t>
         </is>
       </c>
-      <c r="HP2" t="inlineStr">
+      <c r="HA2" t="inlineStr">
         <is>
           <t>week</t>
         </is>
       </c>
-      <c r="IT2" t="inlineStr">
-        <is>
-          <t>visium-v2_coordinates.txt</t>
-        </is>
-      </c>
-      <c r="IU2" t="inlineStr">
-        <is>
-          <t>txt</t>
-        </is>
-      </c>
-      <c r="IV2" t="inlineStr">
-        <is>
-          <t>coordinates list</t>
-        </is>
-      </c>
-      <c r="IW2" t="inlineStr">
-        <is>
-          <t>data:2012</t>
-        </is>
-      </c>
-      <c r="IX2" t="inlineStr">
-        <is>
-          <t>Sequence coordinates</t>
-        </is>
-      </c>
-      <c r="IZ2" t="inlineStr">
-        <is>
-          <t>ArrayExpress</t>
-        </is>
-      </c>
-      <c r="JB2" t="inlineStr">
-        <is>
-          <t>Visiumanalysis</t>
-        </is>
-      </c>
-      <c r="JD2" t="inlineStr">
-        <is>
-          <t>HumanVisiumLibraryPrep</t>
-        </is>
-      </c>
-      <c r="JE2" t="inlineStr">
-        <is>
-          <t>HumanVisiumSequencing</t>
+      <c r="IE2" t="inlineStr">
+        <is>
+          <t>['F78-14789']</t>
         </is>
       </c>
     </row>
@@ -2230,298 +2104,242 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
+          <t>['6330STDY9479160imagespecimen']</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
           <t>6330STDY9479160imagespecimen</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>6330STDY9479160imagespecimen</t>
         </is>
       </c>
-      <c r="AD3" t="n">
+      <c r="AE3" t="n">
         <v>9606</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AL3" t="n">
         <v>10</v>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="AP3" t="inlineStr">
         <is>
           <t>6330STDY9479160specimen</t>
         </is>
       </c>
-      <c r="AP3" t="inlineStr">
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>HumanVisiumSpatialLibraryPrep</t>
         </is>
       </c>
-      <c r="BG3" t="inlineStr">
-        <is>
-          <t>VisiumImagingProtocol</t>
-        </is>
-      </c>
       <c r="BH3" t="inlineStr">
         <is>
-          <t>All images for this process were scanned x40 on Hamamatsu NanoZoomer S60.</t>
+          <t>['6330STDY9479160imagespecimen']</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>6330STDY9479160specimen</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>HumanFetalVisium</t>
+        </is>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>F102</t>
+        </is>
+      </c>
+      <c r="BL3" t="inlineStr">
+        <is>
+          <t>HumanVisiumCollection</t>
         </is>
       </c>
       <c r="BM3" t="inlineStr">
         <is>
-          <t>fluorescence microscopy</t>
-        </is>
-      </c>
-      <c r="BN3" t="inlineStr">
-        <is>
-          <t>FBbi:00000246</t>
-        </is>
-      </c>
-      <c r="BO3" t="inlineStr">
-        <is>
-          <t>fluorescence microscopy</t>
-        </is>
-      </c>
-      <c r="BP3" t="inlineStr">
-        <is>
-          <t>40x</t>
-        </is>
-      </c>
-      <c r="BQ3" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="BT3" t="n">
-        <v>230</v>
+          <t>F102-FPIL-0-FO-1-S4</t>
+        </is>
+      </c>
+      <c r="BN3" t="n">
+        <v>9606</v>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>NCBITaxon:9606</t>
+        </is>
+      </c>
+      <c r="BV3" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="BW3" t="inlineStr">
+        <is>
+          <t>small intestine</t>
+        </is>
+      </c>
+      <c r="BX3" t="inlineStr">
+        <is>
+          <t>UBERON:0002108</t>
+        </is>
+      </c>
+      <c r="BY3" t="inlineStr">
+        <is>
+          <t>small intestine</t>
+        </is>
       </c>
       <c r="BZ3" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>proximal ileum</t>
         </is>
       </c>
       <c r="CA3" t="inlineStr">
         <is>
-          <t>6330STDY9479160specimen</t>
+          <t>FMA:14964</t>
         </is>
       </c>
       <c r="CB3" t="inlineStr">
         <is>
+          <t>Proximal part of ileum</t>
+        </is>
+      </c>
+      <c r="DQ3" t="inlineStr">
+        <is>
+          <t>['6330STDY9479160specimen']</t>
+        </is>
+      </c>
+      <c r="DS3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> All tissues were sectioned using the Leica CX3050S cryostat and were cut at 10um. Tissue optimization was performed to obtain permeabilization time for fetal tissue (12 min).</t>
+        </is>
+      </c>
+      <c r="EP3" t="inlineStr">
+        <is>
+          <t>['HumanVisiumSpatialLibraryPrep']</t>
+        </is>
+      </c>
+      <c r="ER3" t="inlineStr">
+        <is>
+          <t>Human fetal tissues were obtained from the MRC/Wellcome Trust-funded Human Developmental Biology Resource(HDBR, http://www.hdbr.org) with appropriate maternal written consent and approval from the Newcastle and North Tyneside NHS Health Authority Joint Ethics Committee (08/H0906/21+5). All tissues were processed immediately after isolation using consistent protocols with variation in enzymatic digestion strength. Samples were embedded in OCT, either in a mould or on a piece of cork, either over dry ice or in a liquid nitrogen bath.</t>
+        </is>
+      </c>
+      <c r="EV3" t="inlineStr">
+        <is>
+          <t>collecting specimen from organ postmortem</t>
+        </is>
+      </c>
+      <c r="EW3" t="inlineStr">
+        <is>
+          <t>EFO:0009627</t>
+        </is>
+      </c>
+      <c r="EX3" t="inlineStr">
+        <is>
+          <t>collecting specimen from organ postmortem</t>
+        </is>
+      </c>
+      <c r="FE3" t="inlineStr">
+        <is>
+          <t>['HumanVisiumCollection']</t>
+        </is>
+      </c>
+      <c r="FF3" t="inlineStr">
+        <is>
+          <t>F102</t>
+        </is>
+      </c>
+      <c r="FG3" t="inlineStr">
+        <is>
           <t>HumanFetalVisium</t>
         </is>
       </c>
-      <c r="CC3" t="inlineStr">
-        <is>
-          <t>F102</t>
-        </is>
-      </c>
-      <c r="CD3" t="inlineStr">
-        <is>
-          <t>HumanVisiumCollection</t>
-        </is>
-      </c>
-      <c r="CE3" t="inlineStr">
-        <is>
-          <t>F102-FPIL-0-FO-1-S4</t>
-        </is>
-      </c>
-      <c r="CF3" t="n">
+      <c r="FI3" t="n">
         <v>9606</v>
       </c>
-      <c r="CL3" t="inlineStr">
+      <c r="FV3" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="CM3" t="inlineStr">
+      <c r="FW3" t="inlineStr">
         <is>
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="CN3" t="inlineStr">
+      <c r="FX3" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="CO3" t="inlineStr">
-        <is>
-          <t>small intestine</t>
-        </is>
-      </c>
-      <c r="CP3" t="inlineStr">
-        <is>
-          <t>UBERON:0002108</t>
-        </is>
-      </c>
-      <c r="CQ3" t="inlineStr">
-        <is>
-          <t>small intestine</t>
-        </is>
-      </c>
-      <c r="CR3" t="inlineStr">
-        <is>
-          <t>proximal ileum</t>
-        </is>
-      </c>
-      <c r="CS3" t="inlineStr">
-        <is>
-          <t>FMA:14964</t>
-        </is>
-      </c>
-      <c r="CT3" t="inlineStr">
-        <is>
-          <t>Proximal part of ileum</t>
-        </is>
-      </c>
-      <c r="EJ3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> All tissues were sectioned using the Leica CX3050S cryostat and were cut at 10um. Tissue optimization was performed to obtain permeabilization time for fetal tissue (12 min).</t>
-        </is>
-      </c>
-      <c r="FH3" t="inlineStr">
-        <is>
-          <t>Human fetal tissues were obtained from the MRC/Wellcome Trust-funded Human Developmental Biology Resource(HDBR, http://www.hdbr.org) with appropriate maternal written consent and approval from the Newcastle and North Tyneside NHS Health Authority Joint Ethics Committee (08/H0906/21+5). All tissues were processed immediately after isolation using consistent protocols with variation in enzymatic digestion strength. Samples were embedded in OCT, either in a mould or on a piece of cork, either over dry ice or in a liquid nitrogen bath.</t>
-        </is>
-      </c>
-      <c r="FL3" t="inlineStr">
-        <is>
-          <t>collecting specimen from organ postmortem</t>
-        </is>
-      </c>
-      <c r="FM3" t="inlineStr">
-        <is>
-          <t>EFO:0009627</t>
-        </is>
-      </c>
-      <c r="FN3" t="inlineStr">
-        <is>
-          <t>collecting specimen from organ postmortem</t>
-        </is>
-      </c>
-      <c r="FU3" t="inlineStr">
-        <is>
-          <t>F102</t>
-        </is>
-      </c>
-      <c r="FV3" t="inlineStr">
-        <is>
-          <t>HumanFetalVisium</t>
-        </is>
-      </c>
-      <c r="FX3" t="n">
-        <v>9606</v>
-      </c>
-      <c r="GK3" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="GL3" t="inlineStr">
-        <is>
-          <t>NCBITaxon:9606</t>
-        </is>
-      </c>
-      <c r="GM3" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="GN3" t="inlineStr">
+      <c r="FY3" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="GO3" t="inlineStr">
+      <c r="FZ3" t="inlineStr">
         <is>
           <t>not applicable</t>
         </is>
       </c>
-      <c r="GT3" t="inlineStr">
+      <c r="GE3" t="inlineStr">
         <is>
           <t>embryo</t>
         </is>
       </c>
-      <c r="GU3" t="inlineStr">
+      <c r="GF3" t="inlineStr">
         <is>
           <t>UBERON:0000068</t>
         </is>
       </c>
-      <c r="GV3" t="inlineStr">
+      <c r="GG3" t="inlineStr">
         <is>
           <t>embryo stage</t>
         </is>
       </c>
-      <c r="GW3" t="inlineStr">
+      <c r="GH3" t="inlineStr">
         <is>
           <t>normal</t>
         </is>
       </c>
-      <c r="GX3" t="inlineStr">
+      <c r="GI3" t="inlineStr">
         <is>
           <t>PATO:0000461</t>
         </is>
       </c>
+      <c r="GJ3" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="GX3" t="n">
+        <v>17</v>
+      </c>
       <c r="GY3" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="HM3" t="n">
-        <v>17</v>
-      </c>
-      <c r="HN3" t="inlineStr">
-        <is>
           <t>week</t>
         </is>
       </c>
-      <c r="HO3" t="inlineStr">
+      <c r="GZ3" t="inlineStr">
         <is>
           <t>UO:0000034</t>
         </is>
       </c>
-      <c r="HP3" t="inlineStr">
+      <c r="HA3" t="inlineStr">
         <is>
           <t>week</t>
         </is>
       </c>
-      <c r="IT3" t="inlineStr">
-        <is>
-          <t>visium-v2_coordinates.txt</t>
-        </is>
-      </c>
-      <c r="IU3" t="inlineStr">
-        <is>
-          <t>txt</t>
-        </is>
-      </c>
-      <c r="IV3" t="inlineStr">
-        <is>
-          <t>coordinates list</t>
-        </is>
-      </c>
-      <c r="IW3" t="inlineStr">
-        <is>
-          <t>data:2012</t>
-        </is>
-      </c>
-      <c r="IX3" t="inlineStr">
-        <is>
-          <t>Sequence coordinates</t>
-        </is>
-      </c>
-      <c r="IZ3" t="inlineStr">
-        <is>
-          <t>ArrayExpress</t>
-        </is>
-      </c>
-      <c r="JB3" t="inlineStr">
-        <is>
-          <t>Visiumanalysis</t>
-        </is>
-      </c>
-      <c r="JD3" t="inlineStr">
-        <is>
-          <t>HumanVisiumLibraryPrep</t>
-        </is>
-      </c>
-      <c r="JE3" t="inlineStr">
-        <is>
-          <t>HumanVisiumSequencing</t>
+      <c r="IE3" t="inlineStr">
+        <is>
+          <t>['F102']</t>
         </is>
       </c>
     </row>
@@ -2571,298 +2389,242 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
+          <t>['6330STDY9479163imagespecimen']</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
           <t>6330STDY9479163imagespecimen</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>6330STDY9479163imagespecimen</t>
         </is>
       </c>
-      <c r="AD4" t="n">
+      <c r="AE4" t="n">
         <v>9606</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AL4" t="n">
         <v>10</v>
       </c>
-      <c r="AO4" t="inlineStr">
+      <c r="AP4" t="inlineStr">
         <is>
           <t>6330STDY9479163specimen</t>
         </is>
       </c>
-      <c r="AP4" t="inlineStr">
+      <c r="AQ4" t="inlineStr">
         <is>
           <t>HumanVisiumSpatialLibraryPrep</t>
         </is>
       </c>
-      <c r="BG4" t="inlineStr">
-        <is>
-          <t>VisiumImagingProtocol</t>
-        </is>
-      </c>
       <c r="BH4" t="inlineStr">
         <is>
-          <t>All images for this process were scanned x40 on Hamamatsu NanoZoomer S60.</t>
+          <t>['6330STDY9479163imagespecimen']</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>6330STDY9479163specimen</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr">
+        <is>
+          <t>HumanFetalVisium</t>
+        </is>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>sst1</t>
+        </is>
+      </c>
+      <c r="BL4" t="inlineStr">
+        <is>
+          <t>HumanVisiumCollection</t>
         </is>
       </c>
       <c r="BM4" t="inlineStr">
         <is>
-          <t>fluorescence microscopy</t>
-        </is>
-      </c>
-      <c r="BN4" t="inlineStr">
-        <is>
-          <t>FBbi:00000246</t>
-        </is>
-      </c>
-      <c r="BO4" t="inlineStr">
-        <is>
-          <t>fluorescence microscopy</t>
-        </is>
-      </c>
-      <c r="BP4" t="inlineStr">
-        <is>
-          <t>40x</t>
-        </is>
-      </c>
-      <c r="BQ4" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="BT4" t="n">
-        <v>230</v>
+          <t>Sst1-FLI-0-FO-2-S4</t>
+        </is>
+      </c>
+      <c r="BN4" t="n">
+        <v>9606</v>
+      </c>
+      <c r="BT4" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>NCBITaxon:9606</t>
+        </is>
+      </c>
+      <c r="BV4" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="BW4" t="inlineStr">
+        <is>
+          <t>large intestine</t>
+        </is>
+      </c>
+      <c r="BX4" t="inlineStr">
+        <is>
+          <t>UBERON:0000059</t>
+        </is>
+      </c>
+      <c r="BY4" t="inlineStr">
+        <is>
+          <t>large intestine</t>
+        </is>
       </c>
       <c r="BZ4" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>large intestine</t>
         </is>
       </c>
       <c r="CA4" t="inlineStr">
         <is>
-          <t>6330STDY9479163specimen</t>
+          <t>UBERON:0000059</t>
         </is>
       </c>
       <c r="CB4" t="inlineStr">
         <is>
+          <t>large intestine</t>
+        </is>
+      </c>
+      <c r="DQ4" t="inlineStr">
+        <is>
+          <t>['6330STDY9479163specimen']</t>
+        </is>
+      </c>
+      <c r="DS4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> All tissues were sectioned using the Leica CX3050S cryostat and were cut at 10um. Tissue optimization was performed to obtain permeabilization time for fetal tissue (12 min).</t>
+        </is>
+      </c>
+      <c r="EP4" t="inlineStr">
+        <is>
+          <t>['HumanVisiumSpatialLibraryPrep']</t>
+        </is>
+      </c>
+      <c r="ER4" t="inlineStr">
+        <is>
+          <t>Human fetal tissues were obtained from the MRC/Wellcome Trust-funded Human Developmental Biology Resource(HDBR, http://www.hdbr.org) with appropriate maternal written consent and approval from the Newcastle and North Tyneside NHS Health Authority Joint Ethics Committee (08/H0906/21+5). All tissues were processed immediately after isolation using consistent protocols with variation in enzymatic digestion strength. Samples were embedded in OCT, either in a mould or on a piece of cork, either over dry ice or in a liquid nitrogen bath.</t>
+        </is>
+      </c>
+      <c r="EV4" t="inlineStr">
+        <is>
+          <t>collecting specimen from organ postmortem</t>
+        </is>
+      </c>
+      <c r="EW4" t="inlineStr">
+        <is>
+          <t>EFO:0009627</t>
+        </is>
+      </c>
+      <c r="EX4" t="inlineStr">
+        <is>
+          <t>collecting specimen from organ postmortem</t>
+        </is>
+      </c>
+      <c r="FE4" t="inlineStr">
+        <is>
+          <t>['HumanVisiumCollection']</t>
+        </is>
+      </c>
+      <c r="FF4" t="inlineStr">
+        <is>
+          <t>sst1</t>
+        </is>
+      </c>
+      <c r="FG4" t="inlineStr">
+        <is>
           <t>HumanFetalVisium</t>
         </is>
       </c>
-      <c r="CC4" t="inlineStr">
-        <is>
-          <t>sst1</t>
-        </is>
-      </c>
-      <c r="CD4" t="inlineStr">
-        <is>
-          <t>HumanVisiumCollection</t>
-        </is>
-      </c>
-      <c r="CE4" t="inlineStr">
-        <is>
-          <t>Sst1-FLI-0-FO-2-S4</t>
-        </is>
-      </c>
-      <c r="CF4" t="n">
+      <c r="FI4" t="n">
         <v>9606</v>
       </c>
-      <c r="CL4" t="inlineStr">
+      <c r="FV4" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="CM4" t="inlineStr">
+      <c r="FW4" t="inlineStr">
         <is>
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="CN4" t="inlineStr">
+      <c r="FX4" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="CO4" t="inlineStr">
-        <is>
-          <t>large intestine</t>
-        </is>
-      </c>
-      <c r="CP4" t="inlineStr">
-        <is>
-          <t>UBERON:0000059</t>
-        </is>
-      </c>
-      <c r="CQ4" t="inlineStr">
-        <is>
-          <t>large intestine</t>
-        </is>
-      </c>
-      <c r="CR4" t="inlineStr">
-        <is>
-          <t>large intestine</t>
-        </is>
-      </c>
-      <c r="CS4" t="inlineStr">
-        <is>
-          <t>UBERON:0000059</t>
-        </is>
-      </c>
-      <c r="CT4" t="inlineStr">
-        <is>
-          <t>large intestine</t>
-        </is>
-      </c>
-      <c r="EJ4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> All tissues were sectioned using the Leica CX3050S cryostat and were cut at 10um. Tissue optimization was performed to obtain permeabilization time for fetal tissue (12 min).</t>
-        </is>
-      </c>
-      <c r="FH4" t="inlineStr">
-        <is>
-          <t>Human fetal tissues were obtained from the MRC/Wellcome Trust-funded Human Developmental Biology Resource(HDBR, http://www.hdbr.org) with appropriate maternal written consent and approval from the Newcastle and North Tyneside NHS Health Authority Joint Ethics Committee (08/H0906/21+5). All tissues were processed immediately after isolation using consistent protocols with variation in enzymatic digestion strength. Samples were embedded in OCT, either in a mould or on a piece of cork, either over dry ice or in a liquid nitrogen bath.</t>
-        </is>
-      </c>
-      <c r="FL4" t="inlineStr">
-        <is>
-          <t>collecting specimen from organ postmortem</t>
-        </is>
-      </c>
-      <c r="FM4" t="inlineStr">
-        <is>
-          <t>EFO:0009627</t>
-        </is>
-      </c>
-      <c r="FN4" t="inlineStr">
-        <is>
-          <t>collecting specimen from organ postmortem</t>
-        </is>
-      </c>
-      <c r="FU4" t="inlineStr">
-        <is>
-          <t>sst1</t>
-        </is>
-      </c>
-      <c r="FV4" t="inlineStr">
-        <is>
-          <t>HumanFetalVisium</t>
-        </is>
-      </c>
-      <c r="FX4" t="n">
-        <v>9606</v>
-      </c>
-      <c r="GK4" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="GL4" t="inlineStr">
-        <is>
-          <t>NCBITaxon:9606</t>
-        </is>
-      </c>
-      <c r="GM4" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="GN4" t="inlineStr">
+      <c r="FY4" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="GO4" t="inlineStr">
+      <c r="FZ4" t="inlineStr">
         <is>
           <t>not applicable</t>
         </is>
       </c>
-      <c r="GT4" t="inlineStr">
+      <c r="GE4" t="inlineStr">
         <is>
           <t>embryo</t>
         </is>
       </c>
-      <c r="GU4" t="inlineStr">
+      <c r="GF4" t="inlineStr">
         <is>
           <t>UBERON:0000068</t>
         </is>
       </c>
-      <c r="GV4" t="inlineStr">
+      <c r="GG4" t="inlineStr">
         <is>
           <t>embryo stage</t>
         </is>
       </c>
-      <c r="GW4" t="inlineStr">
+      <c r="GH4" t="inlineStr">
         <is>
           <t>normal</t>
         </is>
       </c>
-      <c r="GX4" t="inlineStr">
+      <c r="GI4" t="inlineStr">
         <is>
           <t>PATO:0000461</t>
         </is>
       </c>
+      <c r="GJ4" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="GX4" t="n">
+        <v>13</v>
+      </c>
       <c r="GY4" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="HM4" t="n">
-        <v>13</v>
-      </c>
-      <c r="HN4" t="inlineStr">
-        <is>
           <t>week</t>
         </is>
       </c>
-      <c r="HO4" t="inlineStr">
+      <c r="GZ4" t="inlineStr">
         <is>
           <t>UO:0000034</t>
         </is>
       </c>
-      <c r="HP4" t="inlineStr">
+      <c r="HA4" t="inlineStr">
         <is>
           <t>week</t>
         </is>
       </c>
-      <c r="IT4" t="inlineStr">
-        <is>
-          <t>visium-v2_coordinates.txt</t>
-        </is>
-      </c>
-      <c r="IU4" t="inlineStr">
-        <is>
-          <t>txt</t>
-        </is>
-      </c>
-      <c r="IV4" t="inlineStr">
-        <is>
-          <t>coordinates list</t>
-        </is>
-      </c>
-      <c r="IW4" t="inlineStr">
-        <is>
-          <t>data:2012</t>
-        </is>
-      </c>
-      <c r="IX4" t="inlineStr">
-        <is>
-          <t>Sequence coordinates</t>
-        </is>
-      </c>
-      <c r="IZ4" t="inlineStr">
-        <is>
-          <t>ArrayExpress</t>
-        </is>
-      </c>
-      <c r="JB4" t="inlineStr">
-        <is>
-          <t>Visiumanalysis</t>
-        </is>
-      </c>
-      <c r="JD4" t="inlineStr">
-        <is>
-          <t>HumanVisiumLibraryPrep</t>
-        </is>
-      </c>
-      <c r="JE4" t="inlineStr">
-        <is>
-          <t>HumanVisiumSequencing</t>
+      <c r="IE4" t="inlineStr">
+        <is>
+          <t>['sst1']</t>
         </is>
       </c>
     </row>

</xml_diff>